<commit_message>
MODIFY Usecase.xlsx add new use case
</commit_message>
<xml_diff>
--- a/Project Design/Usecase.xlsx
+++ b/Project Design/Usecase.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Usecase Tempalte" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Use Case ID:</t>
   </si>
@@ -82,6 +82,42 @@
   </si>
   <si>
     <t>3.</t>
+  </si>
+  <si>
+    <t>Thang Le Quoc</t>
+  </si>
+  <si>
+    <t>17/10/2010</t>
+  </si>
+  <si>
+    <t>Request scenario</t>
+  </si>
+  <si>
+    <t>System adminitrator</t>
+  </si>
+  <si>
+    <t>User of the system do a lot of actions that cause IDS agents create series of alerts</t>
+  </si>
+  <si>
+    <t>The system adminitrator click the "view scenario" button in the program</t>
+  </si>
+  <si>
+    <t>1.The admin click the "view scenario" button. The sofware process the request and take the current scenario from correlation engine</t>
+  </si>
+  <si>
+    <t>2.The system call the drawing function to visualize the scenario</t>
+  </si>
+  <si>
+    <t>1.System adminitrator want to view the scenario</t>
+  </si>
+  <si>
+    <t>1.A picture will appear on the screen</t>
+  </si>
+  <si>
+    <t>1. When the system detect an malicious action. It will create an alert for system adminitrator and draw that scenario.</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
 </sst>
 </file>
@@ -92,7 +128,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -101,7 +137,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -110,7 +146,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -251,8 +287,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,21 +305,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -286,6 +313,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,189 +619,193 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.875" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="18.625" customWidth="1"/>
-    <col min="4" max="4" width="30.625" customWidth="1"/>
-    <col min="5" max="5" width="25.125" customWidth="1"/>
-    <col min="6" max="6" width="20.25" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
-      <c r="D1" s="9" t="s">
+    <row r="1" spans="1:5" ht="18.75">
+      <c r="D1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="10" t="s">
+      <c r="E1" s="17"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="11" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="12" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="15">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="11" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="15">
-      <c r="A12" s="11" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="15">
-      <c r="A13" s="11" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" ht="15">
-      <c r="A14" s="11" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="14"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="20" spans="1:4" ht="15">
-      <c r="A20" s="11" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" ht="15">
-      <c r="A21" s="11" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" ht="15">
-      <c r="A22" s="11" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" ht="15">
-      <c r="A23" s="11" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" ht="15">
-      <c r="A24" s="11" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
@@ -782,10 +822,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -794,12 +830,236 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75">
+      <c r="D1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="16"/>
+      <c r="B16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="9"/>
+      <c r="B17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="9"/>
+      <c r="B19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -810,7 +1070,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MODIFY Usecase.xlsx repair the use case
</commit_message>
<xml_diff>
--- a/Project Design/Usecase.xlsx
+++ b/Project Design/Usecase.xlsx
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -867,11 +867,11 @@
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">

</xml_diff>